<commit_message>
Information added to data needed excel
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/ammonia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="13_ncr:1_{B63BCB0A-9012-4F55-92B6-F45564B797E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DB741AE-6A77-4E4B-8874-164E6D011B5A}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="13_ncr:1_{B63BCB0A-9012-4F55-92B6-F45564B797E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86F0E5C2-4972-46A3-8B36-69570E20B2AC}"/>
   <bookViews>
-    <workbookView xWindow="-1560" yWindow="-19440" windowWidth="38700" windowHeight="15315" activeTab="3" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="116">
   <si>
     <t>Unit</t>
   </si>
@@ -419,6 +419,9 @@
   </si>
   <si>
     <t>nh3_st</t>
+  </si>
+  <si>
+    <t>Reformer</t>
   </si>
 </sst>
 </file>
@@ -1363,8 +1366,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5F8A7EB-52A6-4AC4-94D0-FF5952E382A3}" name="Table4" displayName="Table4" ref="A1:A21" totalsRowShown="0">
-  <autoFilter ref="A1:A21" xr:uid="{E5F8A7EB-52A6-4AC4-94D0-FF5952E382A3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5F8A7EB-52A6-4AC4-94D0-FF5952E382A3}" name="Table4" displayName="Table4" ref="A1:A22" totalsRowShown="0">
+  <autoFilter ref="A1:A22" xr:uid="{E5F8A7EB-52A6-4AC4-94D0-FF5952E382A3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{99EC3AFF-E76A-4BF2-94D0-13EEEC46286A}" name="object_type"/>
   </tableColumns>
@@ -1904,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CABA7C5-6230-4207-9D35-0A95D86E66AC}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2593,7 +2596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -2721,10 +2724,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DC79B9-9C58-497E-9FD8-D3F2239E9BDC}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2837,6 +2840,11 @@
         <v>107</v>
       </c>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
update tables and data
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/ammonia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\ammonia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="13_ncr:1_{B63BCB0A-9012-4F55-92B6-F45564B797E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86F0E5C2-4972-46A3-8B36-69570E20B2AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC9FBA7-0C5D-4797-BE21-F108AB144988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="114">
   <si>
     <t>Unit</t>
   </si>
@@ -295,9 +295,6 @@
     <t>water</t>
   </si>
   <si>
-    <t>steam</t>
-  </si>
-  <si>
     <t>steam_plant</t>
   </si>
   <si>
@@ -322,15 +319,9 @@
     <t>heat_high</t>
   </si>
   <si>
-    <t>heat_split</t>
-  </si>
-  <si>
     <t>Auxilliary</t>
   </si>
   <si>
-    <t>internal_heat</t>
-  </si>
-  <si>
     <t>Input3</t>
   </si>
   <si>
@@ -422,6 +413,9 @@
   </si>
   <si>
     <t>Reformer</t>
+  </si>
+  <si>
+    <t>o2</t>
   </si>
 </sst>
 </file>
@@ -1250,10 +1244,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:R11" totalsRowShown="0">
   <autoFilter ref="A1:R11" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
@@ -1282,8 +1272,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}" name="Table5" displayName="Table5" ref="A1:Q12" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="A1:Q12" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}" name="Table5" displayName="Table5" ref="A1:Q10" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="A1:Q10" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{2BE3E317-773B-4E82-9035-69A43C6CB21B}" name="Unit" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{22613EE0-390D-4B04-9A9B-6D5554D1C8ED}" name="Object_type" dataDxfId="18"/>
@@ -1701,7 +1691,7 @@
         <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -1710,16 +1700,16 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J1" t="s">
         <v>61</v>
@@ -1746,7 +1736,7 @@
         <v>41</v>
       </c>
       <c r="R1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -1764,7 +1754,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
@@ -1777,7 +1767,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
         <v>60</v>
@@ -1790,7 +1780,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
         <v>57</v>
@@ -1812,10 +1802,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
         <v>67</v>
@@ -1825,10 +1815,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
         <v>67</v>
@@ -1838,7 +1828,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
@@ -1854,10 +1844,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
         <v>72</v>
@@ -1905,10 +1895,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CABA7C5-6230-4207-9D35-0A95D86E66AC}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1932,10 +1922,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
@@ -1944,31 +1934,31 @@
         <v>4</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -1998,7 +1988,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>59</v>
@@ -2023,7 +2013,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
         <v>60</v>
@@ -2048,7 +2038,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>57</v>
@@ -2062,10 +2052,10 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -2083,10 +2073,10 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>67</v>
@@ -2095,9 +2085,11 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="H6" s="3"/>
+        <v>106</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -2110,26 +2102,26 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>67</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -2143,115 +2135,51 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>72</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="4">
-        <v>7.2437800000000002E-4</v>
-      </c>
+      <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6">
-        <v>1</v>
-      </c>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-    </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4">
-        <v>1</v>
-      </c>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2266,7 +2194,7 @@
           <x14:formula1>
             <xm:f>Drop_Down!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B12 B1:B10</xm:sqref>
+          <xm:sqref>B10 B1:B8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2452,22 +2380,22 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
       </c>
       <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
         <v>75</v>
       </c>
-      <c r="D3" t="s">
-        <v>76</v>
-      </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G3" t="s">
         <v>32</v>
@@ -2508,22 +2436,22 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" t="s">
         <v>111</v>
       </c>
-      <c r="C4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" t="s">
-        <v>114</v>
-      </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G4" t="s">
         <v>32</v>
@@ -2540,7 +2468,7 @@
         <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
         <v>71</v>
@@ -2652,7 +2580,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
@@ -2678,10 +2606,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2777,7 +2705,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
@@ -2807,7 +2735,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
@@ -2827,22 +2755,22 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add relation values to input for ammonia
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\ammonia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC9FBA7-0C5D-4797-BE21-F108AB144988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A398C2-2803-4388-96E0-F2CB59F35ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="114">
   <si>
     <t>Unit</t>
   </si>
@@ -525,20 +525,6 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -573,6 +559,20 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1287,11 +1287,11 @@
     <tableColumn id="10" xr3:uid="{CD6FCAF1-2543-4CF8-99F5-E24DBA2DEDC0}" name="Output4" dataDxfId="10"/>
     <tableColumn id="11" xr3:uid="{88F2DAC4-E2C3-4C34-B709-2523E8BE5B1F}" name="Relation_In1_In2" dataDxfId="9"/>
     <tableColumn id="14" xr3:uid="{3C190E97-FD9A-4F36-8EBF-717B1ECA00B1}" name="Relation_In1_In3" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{043147D8-AE82-457E-8F19-EB4AE9D43B9E}" name="Relation_In1_In4" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{A190E492-7FDF-403D-B8AF-17448A48E47F}" name="Relation_In1_Out1" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{26E8D274-C985-4E20-8920-2BAC0A372552}" name="Relation_Out1_Out2" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{4E0BCAE8-11F8-4D98-AECC-86C8A3C2B5C1}" name="Relation_Out1_Out3" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{3C0369D5-4DD0-4B4B-9480-0C4665C0BC59}" name="Relation_Out1_Out4" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{043147D8-AE82-457E-8F19-EB4AE9D43B9E}" name="Relation_In1_In4" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{A190E492-7FDF-403D-B8AF-17448A48E47F}" name="Relation_In1_Out1" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{26E8D274-C985-4E20-8920-2BAC0A372552}" name="Relation_Out1_Out2" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{4E0BCAE8-11F8-4D98-AECC-86C8A3C2B5C1}" name="Relation_Out1_Out3" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{3C0369D5-4DD0-4B4B-9480-0C4665C0BC59}" name="Relation_Out1_Out4" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1307,7 +1307,7 @@
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -1326,7 +1326,7 @@
     <tableColumn id="21" xr3:uid="{EC2CC790-C17D-4744-A981-3984808E5B33}" name="vom_cost_Input2"/>
     <tableColumn id="24" xr3:uid="{41B338E4-2058-41E9-8000-97D77450FBC3}" name="vom_cost_Output1"/>
     <tableColumn id="25" xr3:uid="{DDAFCF0A-1EF1-4B7B-9742-01F9FA7A22E5}" name="vom_cost_Output2"/>
-    <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime" dataDxfId="1"/>
+    <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime" dataDxfId="2"/>
     <tableColumn id="30" xr3:uid="{09434E4A-7BF5-4547-9708-EA3F0F7ADC8E}" name="initial_connections_invested_available"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1337,7 +1337,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:K5" totalsRowShown="0">
   <autoFilter ref="A1:K5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="1">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{8C29206C-8DC6-44DB-A8D1-3D5625C277AD}" name="Object_type"/>
@@ -1898,7 +1898,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2095,8 +2095,12 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
+      <c r="N6" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="O6" s="3">
+        <v>3.4482758620689657</v>
+      </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
     </row>
@@ -2108,13 +2112,13 @@
         <v>104</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
@@ -2123,14 +2127,26 @@
       <c r="H7" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
+      <c r="K7">
+        <v>17.867924528301888</v>
+      </c>
+      <c r="L7" s="4">
+        <v>53.933348030570251</v>
+      </c>
       <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
+      <c r="N7">
+        <v>1.1506682867557716</v>
+      </c>
+      <c r="O7" s="4">
+        <v>7.6203703703703694</v>
+      </c>
+      <c r="P7" s="4">
+        <v>21.657894736842106</v>
+      </c>
       <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">

</xml_diff>